<commit_message>
Trying new implementation of OptiRR
</commit_message>
<xml_diff>
--- a/python/test.xlsx
+++ b/python/test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Z40\Documents\GitHub\OS_scheduling\python\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23055" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23060" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="18">
   <si>
     <t>Process</t>
   </si>
@@ -68,6 +73,12 @@
   <si>
     <t>RR TQ = 10</t>
   </si>
+  <si>
+    <t>Optimized RR TQ=5</t>
+  </si>
+  <si>
+    <t>RR TQ=5</t>
+  </si>
 </sst>
 </file>
 
@@ -114,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,6 +143,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -409,7 +423,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,34 +431,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BX32"/>
+  <dimension ref="A2:BX45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
+      <selection pane="bottomRight" activeCell="BX44" sqref="BX44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="3.7109375" style="2" customWidth="1"/>
-    <col min="9" max="73" width="3.7109375" style="1"/>
+    <col min="1" max="1" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" style="1" customWidth="1"/>
+    <col min="4" max="8" width="3.7265625" style="2" customWidth="1"/>
+    <col min="9" max="73" width="3.7265625" style="1"/>
     <col min="74" max="74" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="16384" width="3.7109375" style="1"/>
+    <col min="75" max="16384" width="3.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -762,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -841,7 +855,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -893,7 +907,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -948,7 +962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -988,14 +1002,14 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1439,7 +1453,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1590,7 +1604,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1754,7 +1768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1794,14 +1808,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2028,7 +2042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2245,7 +2259,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -2458,7 +2472,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -2605,7 +2619,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -2772,7 +2786,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -2949,12 +2963,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="2">
         <v>1</v>
       </c>
@@ -3173,7 +3187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -3391,7 +3405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -3585,7 +3599,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -3733,7 +3747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -3901,7 +3915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
@@ -4079,7 +4093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4152,12 +4166,2056 @@
       <c r="BW32" s="2"/>
       <c r="BX32" s="2"/>
     </row>
+    <row r="33" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7">
+        <v>2</v>
+      </c>
+      <c r="F33" s="7">
+        <v>3</v>
+      </c>
+      <c r="G33" s="7">
+        <v>4</v>
+      </c>
+      <c r="H33" s="7">
+        <v>5</v>
+      </c>
+      <c r="I33" s="7">
+        <v>6</v>
+      </c>
+      <c r="J33" s="7">
+        <v>7</v>
+      </c>
+      <c r="K33" s="7">
+        <v>8</v>
+      </c>
+      <c r="L33" s="7">
+        <v>9</v>
+      </c>
+      <c r="M33" s="7">
+        <v>10</v>
+      </c>
+      <c r="N33" s="7">
+        <v>11</v>
+      </c>
+      <c r="O33" s="7">
+        <v>12</v>
+      </c>
+      <c r="P33" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>14</v>
+      </c>
+      <c r="R33" s="7">
+        <v>15</v>
+      </c>
+      <c r="S33" s="7">
+        <v>16</v>
+      </c>
+      <c r="T33" s="7">
+        <v>17</v>
+      </c>
+      <c r="U33" s="7">
+        <v>18</v>
+      </c>
+      <c r="V33" s="7">
+        <v>19</v>
+      </c>
+      <c r="W33" s="7">
+        <v>20</v>
+      </c>
+      <c r="X33" s="7">
+        <v>21</v>
+      </c>
+      <c r="Y33" s="7">
+        <v>22</v>
+      </c>
+      <c r="Z33" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA33" s="7">
+        <v>24</v>
+      </c>
+      <c r="AB33" s="7">
+        <v>25</v>
+      </c>
+      <c r="AC33" s="7">
+        <v>26</v>
+      </c>
+      <c r="AD33" s="7">
+        <v>27</v>
+      </c>
+      <c r="AE33" s="7">
+        <v>28</v>
+      </c>
+      <c r="AF33" s="7">
+        <v>29</v>
+      </c>
+      <c r="AG33" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH33" s="7">
+        <v>31</v>
+      </c>
+      <c r="AI33" s="7">
+        <v>32</v>
+      </c>
+      <c r="AJ33" s="7">
+        <v>33</v>
+      </c>
+      <c r="AK33" s="7">
+        <v>34</v>
+      </c>
+      <c r="AL33" s="7">
+        <v>35</v>
+      </c>
+      <c r="AM33" s="7">
+        <v>36</v>
+      </c>
+      <c r="AN33" s="7">
+        <v>37</v>
+      </c>
+      <c r="AO33" s="7">
+        <v>38</v>
+      </c>
+      <c r="AP33" s="7">
+        <v>39</v>
+      </c>
+      <c r="AQ33" s="7">
+        <v>40</v>
+      </c>
+      <c r="AR33" s="7">
+        <v>41</v>
+      </c>
+      <c r="AS33" s="7">
+        <v>42</v>
+      </c>
+      <c r="AT33" s="7">
+        <v>43</v>
+      </c>
+      <c r="AU33" s="7">
+        <v>44</v>
+      </c>
+      <c r="AV33" s="7">
+        <v>45</v>
+      </c>
+      <c r="AW33" s="7">
+        <v>46</v>
+      </c>
+      <c r="AX33" s="7">
+        <v>47</v>
+      </c>
+      <c r="AY33" s="7">
+        <v>48</v>
+      </c>
+      <c r="AZ33" s="7">
+        <v>49</v>
+      </c>
+      <c r="BA33" s="7">
+        <v>50</v>
+      </c>
+      <c r="BB33" s="7">
+        <v>51</v>
+      </c>
+      <c r="BC33" s="7">
+        <v>52</v>
+      </c>
+      <c r="BD33" s="7">
+        <v>53</v>
+      </c>
+      <c r="BE33" s="7">
+        <v>54</v>
+      </c>
+      <c r="BF33" s="7">
+        <v>55</v>
+      </c>
+      <c r="BG33" s="7">
+        <v>56</v>
+      </c>
+      <c r="BH33" s="7">
+        <v>57</v>
+      </c>
+      <c r="BI33" s="7">
+        <v>58</v>
+      </c>
+      <c r="BJ33" s="7">
+        <v>59</v>
+      </c>
+      <c r="BK33" s="7">
+        <v>60</v>
+      </c>
+      <c r="BL33" s="7">
+        <v>61</v>
+      </c>
+      <c r="BM33" s="7">
+        <v>62</v>
+      </c>
+      <c r="BN33" s="7">
+        <v>63</v>
+      </c>
+      <c r="BO33" s="7">
+        <v>64</v>
+      </c>
+      <c r="BP33" s="7">
+        <v>65</v>
+      </c>
+      <c r="BQ33" s="7">
+        <v>66</v>
+      </c>
+      <c r="BR33" s="7">
+        <v>67</v>
+      </c>
+      <c r="BS33" s="7">
+        <v>68</v>
+      </c>
+      <c r="BT33" s="7">
+        <v>69</v>
+      </c>
+      <c r="BU33" s="7"/>
+      <c r="BV33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX33" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="7">
+        <v>22</v>
+      </c>
+      <c r="C34" s="7">
+        <v>5</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="3">
+        <v>22</v>
+      </c>
+      <c r="J34" s="3">
+        <v>21</v>
+      </c>
+      <c r="K34" s="3">
+        <v>20</v>
+      </c>
+      <c r="L34" s="3">
+        <v>19</v>
+      </c>
+      <c r="M34" s="3">
+        <v>18</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV34" s="3">
+        <v>17</v>
+      </c>
+      <c r="AW34" s="3">
+        <v>16</v>
+      </c>
+      <c r="AX34" s="3">
+        <v>15</v>
+      </c>
+      <c r="AY34" s="3">
+        <v>14</v>
+      </c>
+      <c r="AZ34" s="3">
+        <v>13</v>
+      </c>
+      <c r="BA34" s="3">
+        <v>12</v>
+      </c>
+      <c r="BB34" s="3">
+        <v>11</v>
+      </c>
+      <c r="BC34" s="3">
+        <v>10</v>
+      </c>
+      <c r="BD34" s="3">
+        <v>9</v>
+      </c>
+      <c r="BE34" s="3">
+        <v>8</v>
+      </c>
+      <c r="BF34" s="3">
+        <v>7</v>
+      </c>
+      <c r="BG34" s="3">
+        <v>6</v>
+      </c>
+      <c r="BH34" s="3">
+        <v>5</v>
+      </c>
+      <c r="BI34" s="3">
+        <v>4</v>
+      </c>
+      <c r="BJ34" s="3">
+        <v>3</v>
+      </c>
+      <c r="BK34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BL34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BM34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BN34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BO34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BQ34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BR34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BS34" s="3">
+        <v>2</v>
+      </c>
+      <c r="BT34" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV34" s="1">
+        <v>5</v>
+      </c>
+      <c r="BW34" s="1">
+        <v>42</v>
+      </c>
+      <c r="BX34" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="7">
+        <v>18</v>
+      </c>
+      <c r="C35" s="7">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" s="3">
+        <v>18</v>
+      </c>
+      <c r="O35" s="3">
+        <v>17</v>
+      </c>
+      <c r="P35" s="3">
+        <v>16</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>15</v>
+      </c>
+      <c r="R35" s="3">
+        <v>14</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ35" s="3">
+        <v>13</v>
+      </c>
+      <c r="AR35" s="3">
+        <v>12</v>
+      </c>
+      <c r="AS35" s="3">
+        <v>11</v>
+      </c>
+      <c r="AT35" s="3">
+        <v>10</v>
+      </c>
+      <c r="AU35" s="3">
+        <v>9</v>
+      </c>
+      <c r="AV35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BI35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK35" s="3">
+        <v>8</v>
+      </c>
+      <c r="BL35" s="3">
+        <v>7</v>
+      </c>
+      <c r="BM35" s="3">
+        <v>6</v>
+      </c>
+      <c r="BN35" s="3">
+        <v>5</v>
+      </c>
+      <c r="BO35" s="3">
+        <v>4</v>
+      </c>
+      <c r="BP35" s="3">
+        <v>3</v>
+      </c>
+      <c r="BQ35" s="3">
+        <v>2</v>
+      </c>
+      <c r="BR35" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV35" s="1">
+        <v>10</v>
+      </c>
+      <c r="BW35" s="1">
+        <v>44</v>
+      </c>
+      <c r="BX35" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="7">
+        <v>9</v>
+      </c>
+      <c r="C36" s="7">
+        <v>5</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S36" s="3">
+        <v>9</v>
+      </c>
+      <c r="T36" s="3">
+        <v>8</v>
+      </c>
+      <c r="U36" s="3">
+        <v>7</v>
+      </c>
+      <c r="V36" s="3">
+        <v>6</v>
+      </c>
+      <c r="W36" s="3">
+        <v>5</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH36" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI36" s="3">
+        <v>3</v>
+      </c>
+      <c r="AJ36" s="3">
+        <v>2</v>
+      </c>
+      <c r="AK36" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV36" s="1">
+        <v>15</v>
+      </c>
+      <c r="BW36" s="1">
+        <v>20</v>
+      </c>
+      <c r="BX36" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="7">
+        <v>10</v>
+      </c>
+      <c r="C37" s="7">
+        <v>5</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X37" s="3">
+        <v>10</v>
+      </c>
+      <c r="Y37" s="3">
+        <v>9</v>
+      </c>
+      <c r="Z37" s="3">
+        <v>8</v>
+      </c>
+      <c r="AA37" s="3">
+        <v>7</v>
+      </c>
+      <c r="AB37" s="3">
+        <v>6</v>
+      </c>
+      <c r="AC37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL37" s="3">
+        <v>5</v>
+      </c>
+      <c r="AM37" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN37" s="3">
+        <v>3</v>
+      </c>
+      <c r="AO37" s="3">
+        <v>2</v>
+      </c>
+      <c r="AP37" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV37" s="1">
+        <v>20</v>
+      </c>
+      <c r="BW37" s="1">
+        <v>24</v>
+      </c>
+      <c r="BX37" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="7">
+        <v>5</v>
+      </c>
+      <c r="C38" s="7">
+        <v>5</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC38" s="3">
+        <v>5</v>
+      </c>
+      <c r="AD38" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE38" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF38" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG38" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV38" s="1">
+        <v>25</v>
+      </c>
+      <c r="BW38" s="1">
+        <v>20</v>
+      </c>
+      <c r="BX38" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A40" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7">
+        <v>2</v>
+      </c>
+      <c r="F40" s="7">
+        <v>3</v>
+      </c>
+      <c r="G40" s="7">
+        <v>4</v>
+      </c>
+      <c r="H40" s="7">
+        <v>5</v>
+      </c>
+      <c r="I40" s="7">
+        <v>6</v>
+      </c>
+      <c r="J40" s="7">
+        <v>7</v>
+      </c>
+      <c r="K40" s="7">
+        <v>8</v>
+      </c>
+      <c r="L40" s="7">
+        <v>9</v>
+      </c>
+      <c r="M40" s="7">
+        <v>10</v>
+      </c>
+      <c r="N40" s="7">
+        <v>11</v>
+      </c>
+      <c r="O40" s="7">
+        <v>12</v>
+      </c>
+      <c r="P40" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>14</v>
+      </c>
+      <c r="R40" s="7">
+        <v>15</v>
+      </c>
+      <c r="S40" s="7">
+        <v>16</v>
+      </c>
+      <c r="T40" s="7">
+        <v>17</v>
+      </c>
+      <c r="U40" s="7">
+        <v>18</v>
+      </c>
+      <c r="V40" s="7">
+        <v>19</v>
+      </c>
+      <c r="W40" s="7">
+        <v>20</v>
+      </c>
+      <c r="X40" s="7">
+        <v>21</v>
+      </c>
+      <c r="Y40" s="7">
+        <v>22</v>
+      </c>
+      <c r="Z40" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA40" s="7">
+        <v>24</v>
+      </c>
+      <c r="AB40" s="7">
+        <v>25</v>
+      </c>
+      <c r="AC40" s="7">
+        <v>26</v>
+      </c>
+      <c r="AD40" s="7">
+        <v>27</v>
+      </c>
+      <c r="AE40" s="7">
+        <v>28</v>
+      </c>
+      <c r="AF40" s="7">
+        <v>29</v>
+      </c>
+      <c r="AG40" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH40" s="7">
+        <v>31</v>
+      </c>
+      <c r="AI40" s="7">
+        <v>32</v>
+      </c>
+      <c r="AJ40" s="7">
+        <v>33</v>
+      </c>
+      <c r="AK40" s="7">
+        <v>34</v>
+      </c>
+      <c r="AL40" s="7">
+        <v>35</v>
+      </c>
+      <c r="AM40" s="7">
+        <v>36</v>
+      </c>
+      <c r="AN40" s="7">
+        <v>37</v>
+      </c>
+      <c r="AO40" s="7">
+        <v>38</v>
+      </c>
+      <c r="AP40" s="7">
+        <v>39</v>
+      </c>
+      <c r="AQ40" s="7">
+        <v>40</v>
+      </c>
+      <c r="AR40" s="7">
+        <v>41</v>
+      </c>
+      <c r="AS40" s="7">
+        <v>42</v>
+      </c>
+      <c r="AT40" s="7">
+        <v>43</v>
+      </c>
+      <c r="AU40" s="7">
+        <v>44</v>
+      </c>
+      <c r="AV40" s="7">
+        <v>45</v>
+      </c>
+      <c r="AW40" s="7">
+        <v>46</v>
+      </c>
+      <c r="AX40" s="7">
+        <v>47</v>
+      </c>
+      <c r="AY40" s="7">
+        <v>48</v>
+      </c>
+      <c r="AZ40" s="7">
+        <v>49</v>
+      </c>
+      <c r="BA40" s="7">
+        <v>50</v>
+      </c>
+      <c r="BB40" s="7">
+        <v>51</v>
+      </c>
+      <c r="BC40" s="7">
+        <v>52</v>
+      </c>
+      <c r="BD40" s="7">
+        <v>53</v>
+      </c>
+      <c r="BE40" s="7">
+        <v>54</v>
+      </c>
+      <c r="BF40" s="7">
+        <v>55</v>
+      </c>
+      <c r="BG40" s="7">
+        <v>56</v>
+      </c>
+      <c r="BH40" s="7">
+        <v>57</v>
+      </c>
+      <c r="BI40" s="7">
+        <v>58</v>
+      </c>
+      <c r="BJ40" s="7">
+        <v>59</v>
+      </c>
+      <c r="BK40" s="7">
+        <v>60</v>
+      </c>
+      <c r="BL40" s="7">
+        <v>61</v>
+      </c>
+      <c r="BM40" s="7">
+        <v>62</v>
+      </c>
+      <c r="BN40" s="7">
+        <v>63</v>
+      </c>
+      <c r="BO40" s="7">
+        <v>64</v>
+      </c>
+      <c r="BP40" s="7">
+        <v>65</v>
+      </c>
+      <c r="BQ40" s="7">
+        <v>66</v>
+      </c>
+      <c r="BR40" s="7">
+        <v>67</v>
+      </c>
+      <c r="BS40" s="7">
+        <v>68</v>
+      </c>
+      <c r="BT40" s="7">
+        <v>69</v>
+      </c>
+      <c r="BU40" s="7"/>
+      <c r="BV40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW40" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX40" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="7">
+        <v>22</v>
+      </c>
+      <c r="C41" s="7">
+        <v>5</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="3">
+        <v>22</v>
+      </c>
+      <c r="J41" s="3">
+        <v>21</v>
+      </c>
+      <c r="K41" s="3">
+        <v>20</v>
+      </c>
+      <c r="L41" s="3">
+        <v>19</v>
+      </c>
+      <c r="M41" s="3">
+        <v>18</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH41" s="3">
+        <v>17</v>
+      </c>
+      <c r="AI41" s="3">
+        <v>16</v>
+      </c>
+      <c r="AJ41" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK41" s="3">
+        <v>14</v>
+      </c>
+      <c r="AL41" s="3">
+        <v>13</v>
+      </c>
+      <c r="AM41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA41" s="3">
+        <v>12</v>
+      </c>
+      <c r="BB41" s="3">
+        <v>11</v>
+      </c>
+      <c r="BC41" s="3">
+        <v>10</v>
+      </c>
+      <c r="BD41" s="3">
+        <v>9</v>
+      </c>
+      <c r="BE41" s="3">
+        <v>8</v>
+      </c>
+      <c r="BF41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BI41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK41" s="3">
+        <v>7</v>
+      </c>
+      <c r="BL41" s="3">
+        <v>6</v>
+      </c>
+      <c r="BM41" s="3">
+        <v>5</v>
+      </c>
+      <c r="BN41" s="3">
+        <v>4</v>
+      </c>
+      <c r="BO41" s="3">
+        <v>3</v>
+      </c>
+      <c r="BP41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BQ41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BR41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BS41" s="3">
+        <v>2</v>
+      </c>
+      <c r="BT41" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV41" s="1">
+        <v>5</v>
+      </c>
+      <c r="BW41" s="1">
+        <v>42</v>
+      </c>
+      <c r="BX41" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="7">
+        <v>18</v>
+      </c>
+      <c r="C42" s="7">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N42" s="3">
+        <v>18</v>
+      </c>
+      <c r="O42" s="3">
+        <v>17</v>
+      </c>
+      <c r="P42" s="3">
+        <v>16</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>15</v>
+      </c>
+      <c r="R42" s="3">
+        <v>14</v>
+      </c>
+      <c r="S42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM42" s="3">
+        <v>13</v>
+      </c>
+      <c r="AN42" s="3">
+        <v>12</v>
+      </c>
+      <c r="AO42" s="3">
+        <v>11</v>
+      </c>
+      <c r="AP42" s="3">
+        <v>10</v>
+      </c>
+      <c r="AQ42" s="3">
+        <v>9</v>
+      </c>
+      <c r="AR42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF42" s="3">
+        <v>8</v>
+      </c>
+      <c r="BG42" s="3">
+        <v>7</v>
+      </c>
+      <c r="BH42" s="3">
+        <v>6</v>
+      </c>
+      <c r="BI42" s="3">
+        <v>5</v>
+      </c>
+      <c r="BJ42" s="3">
+        <v>4</v>
+      </c>
+      <c r="BK42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BL42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BM42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BN42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BO42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP42" s="3">
+        <v>3</v>
+      </c>
+      <c r="BQ42" s="3">
+        <v>2</v>
+      </c>
+      <c r="BR42" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV42" s="1">
+        <v>10</v>
+      </c>
+      <c r="BW42" s="1">
+        <v>44</v>
+      </c>
+      <c r="BX42" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="7">
+        <v>9</v>
+      </c>
+      <c r="C43" s="7">
+        <v>5</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S43" s="3">
+        <v>9</v>
+      </c>
+      <c r="T43" s="3">
+        <v>8</v>
+      </c>
+      <c r="U43" s="3">
+        <v>7</v>
+      </c>
+      <c r="V43" s="3">
+        <v>6</v>
+      </c>
+      <c r="W43" s="3">
+        <v>5</v>
+      </c>
+      <c r="X43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR43" s="3">
+        <v>4</v>
+      </c>
+      <c r="AS43" s="3">
+        <v>3</v>
+      </c>
+      <c r="AT43" s="3">
+        <v>2</v>
+      </c>
+      <c r="AU43" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV43" s="1">
+        <v>15</v>
+      </c>
+      <c r="BW43" s="1">
+        <v>30</v>
+      </c>
+      <c r="BX43" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="7">
+        <v>10</v>
+      </c>
+      <c r="C44" s="7">
+        <v>5</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X44" s="3">
+        <v>10</v>
+      </c>
+      <c r="Y44" s="3">
+        <v>9</v>
+      </c>
+      <c r="Z44" s="3">
+        <v>8</v>
+      </c>
+      <c r="AA44" s="3">
+        <v>7</v>
+      </c>
+      <c r="AB44" s="3">
+        <v>6</v>
+      </c>
+      <c r="AC44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV44" s="3">
+        <v>5</v>
+      </c>
+      <c r="AW44" s="3">
+        <v>4</v>
+      </c>
+      <c r="AX44" s="3">
+        <v>3</v>
+      </c>
+      <c r="AY44" s="3">
+        <v>2</v>
+      </c>
+      <c r="AZ44" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV44" s="1">
+        <v>20</v>
+      </c>
+      <c r="BW44" s="1">
+        <v>34</v>
+      </c>
+      <c r="BX44" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="7">
+        <v>5</v>
+      </c>
+      <c r="C45" s="7">
+        <v>5</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC45" s="3">
+        <v>5</v>
+      </c>
+      <c r="AD45" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE45" s="3">
+        <v>3</v>
+      </c>
+      <c r="AF45" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG45" s="3">
+        <v>1</v>
+      </c>
+      <c r="BV45" s="1">
+        <v>25</v>
+      </c>
+      <c r="BW45" s="1">
+        <v>20</v>
+      </c>
+      <c r="BX45" s="1">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A33:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>